<commit_message>
added more dry weights
</commit_message>
<xml_diff>
--- a/litter_traps/litter_dry_weights.xlsx
+++ b/litter_traps/litter_dry_weights.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Oak</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>End date</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Hawthorn</t>
+  </si>
+  <si>
+    <t>Willow</t>
+  </si>
+  <si>
+    <t>Beech</t>
   </si>
 </sst>
 </file>
@@ -89,10 +104,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,19 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -412,25 +428,32 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:20">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -444,35 +467,53 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2">
+    <row r="3" spans="1:20">
+      <c r="A3" s="1">
         <v>42233</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>42255</v>
       </c>
       <c r="C3">
@@ -488,35 +529,240 @@
         <v>0.73</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0.03</v>
-      </c>
-      <c r="H3">
-        <v>0.54</v>
-      </c>
-      <c r="I3">
-        <v>0.7</v>
       </c>
       <c r="J3">
         <v>0.54</v>
       </c>
       <c r="K3">
+        <v>0.7</v>
+      </c>
+      <c r="L3">
+        <v>0.54</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
         <v>1.05</v>
       </c>
-      <c r="L3">
+      <c r="P3">
         <v>0.2</v>
       </c>
-      <c r="M3">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>2.08</v>
       </c>
-      <c r="N3">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42275</v>
+      </c>
+      <c r="C4">
+        <v>1.6</v>
+      </c>
+      <c r="D4">
+        <v>1.57</v>
+      </c>
+      <c r="E4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F4">
+        <v>1.18</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.69</v>
+      </c>
+      <c r="K4">
+        <v>0.61</v>
+      </c>
+      <c r="L4">
+        <v>0.35</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O4">
+        <v>1.97</v>
+      </c>
+      <c r="P4">
+        <v>0.18</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0.89</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="1">
+        <v>42275</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42292</v>
+      </c>
+      <c r="C5">
+        <v>5.25</v>
+      </c>
+      <c r="D5">
+        <v>5.12</v>
+      </c>
+      <c r="E5">
+        <v>4.84</v>
+      </c>
+      <c r="F5">
+        <v>2.93</v>
+      </c>
+      <c r="G5">
+        <v>0.44</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.44</v>
+      </c>
+      <c r="J5">
+        <v>1.77</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>5.36</v>
+      </c>
+      <c r="M5">
+        <v>0.27</v>
+      </c>
+      <c r="N5">
+        <v>0.26</v>
+      </c>
+      <c r="O5">
+        <v>6.14</v>
+      </c>
+      <c r="P5">
+        <v>0.73</v>
+      </c>
+      <c r="Q5">
+        <v>0.26</v>
+      </c>
+      <c r="R5">
+        <v>4.55</v>
+      </c>
+      <c r="S5">
+        <v>0.3</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="1">
+        <v>42292</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42306</v>
+      </c>
+      <c r="C6">
+        <v>11.73</v>
+      </c>
+      <c r="D6">
+        <v>12.47</v>
+      </c>
+      <c r="E6">
+        <v>12.14</v>
+      </c>
+      <c r="F6">
+        <v>2.44</v>
+      </c>
+      <c r="G6">
+        <v>0.4</v>
+      </c>
+      <c r="H6">
+        <v>1.02</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="J6">
+        <v>8.35</v>
+      </c>
+      <c r="K6">
+        <v>11.34</v>
+      </c>
+      <c r="L6">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="M6">
+        <v>2.23</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>10.67</v>
+      </c>
+      <c r="P6">
+        <v>1.84</v>
+      </c>
+      <c r="Q6">
+        <v>2.08</v>
+      </c>
+      <c r="R6">
+        <v>12.03</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:L1"/>
+  <mergeCells count="4">
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added litter dry weights and areas
</commit_message>
<xml_diff>
--- a/litter_traps/litter_dry_weights.xlsx
+++ b/litter_traps/litter_dry_weights.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Oak</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Beech</t>
+  </si>
+  <si>
+    <t>Blackthorn</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,9 +416,10 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -442,18 +446,19 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="2"/>
       <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -488,28 +493,31 @@
         <v>14</v>
       </c>
       <c r="N2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>0</v>
-      </c>
       <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
-        <v>0</v>
-      </c>
       <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>42233</v>
       </c>
@@ -553,25 +561,28 @@
         <v>0</v>
       </c>
       <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1.05</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.2</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>2.08</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>42255</v>
       </c>
@@ -612,28 +623,31 @@
         <v>0</v>
       </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1.97</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.18</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.5</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.89</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
       <c r="T4">
         <v>0</v>
       </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>42275</v>
       </c>
@@ -674,28 +688,31 @@
         <v>0.27</v>
       </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>0.26</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>6.14</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.73</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.26</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>4.55</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>0.3</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>42292</v>
       </c>
@@ -739,30 +756,98 @@
         <v>0</v>
       </c>
       <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>10.67</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1.84</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>2.08</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>12.03</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
       <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="1">
+        <v>42306</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42313</v>
+      </c>
+      <c r="C7">
+        <v>12.8</v>
+      </c>
+      <c r="D7">
+        <v>21.47</v>
+      </c>
+      <c r="E7">
+        <v>17.86</v>
+      </c>
+      <c r="F7">
+        <v>2.56</v>
+      </c>
+      <c r="G7">
+        <v>1.62</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.88</v>
+      </c>
+      <c r="J7">
+        <v>13.53</v>
+      </c>
+      <c r="K7">
+        <v>9.67</v>
+      </c>
+      <c r="L7">
+        <v>0.42</v>
+      </c>
+      <c r="M7">
+        <v>0.34</v>
+      </c>
+      <c r="N7">
+        <v>0.41</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>10.27</v>
+      </c>
+      <c r="Q7">
+        <v>0.76</v>
+      </c>
+      <c r="R7">
+        <v>1.17</v>
+      </c>
+      <c r="S7">
+        <v>14.91</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>